<commit_message>
- updated the people_search_terms test data to include single_user_add test cases - changed a test site because one of the existing test sites is no longer working due to course being concluded.
</commit_message>
<xml_diff>
--- a/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
+++ b/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ely817/tlt/canvas_account_admin_tools/selenium_tests/course_info/test_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-10340" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="-15440" yWindow="-21940" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,18 +12,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>test_case_id</t>
   </si>
@@ -39,18 +34,6 @@
     <t xml:space="preserve">role_id </t>
   </si>
   <si>
-    <t>successful_add</t>
-  </si>
-  <si>
-    <t>['aa000gc0', 'aa000fcz']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guest </t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>Guest</t>
   </si>
   <si>
@@ -79,13 +62,145 @@
   </si>
   <si>
     <t>failures expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_student </t>
+  </si>
+  <si>
+    <t>aa000fre</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>singleuseradd_course_head</t>
+  </si>
+  <si>
+    <t>aa000fsf</t>
+  </si>
+  <si>
+    <t>Course Head</t>
+  </si>
+  <si>
+    <t>singleuseradd_faculty</t>
+  </si>
+  <si>
+    <t>aa000ftg</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_teaching fellow </t>
+  </si>
+  <si>
+    <t>aa000fuh</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_designer </t>
+  </si>
+  <si>
+    <t>aa000fvi</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>singleuseradd_teacher</t>
+  </si>
+  <si>
+    <t>aa000fwj</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>singleuseradd_guest</t>
+  </si>
+  <si>
+    <t>aa000fxk</t>
+  </si>
+  <si>
+    <t>singleuseradd_course_support_staff</t>
+  </si>
+  <si>
+    <t>aa000fyl</t>
+  </si>
+  <si>
+    <t>Course Support Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_teaching staff </t>
+  </si>
+  <si>
+    <t>aa000fzm</t>
+  </si>
+  <si>
+    <t>Teaching Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_shopper </t>
+  </si>
+  <si>
+    <t>aa000g0l</t>
+  </si>
+  <si>
+    <t>Shopper</t>
+  </si>
+  <si>
+    <t>singleuseradd_observer</t>
+  </si>
+  <si>
+    <t>aa000g1m</t>
+  </si>
+  <si>
+    <t>Observer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_guest_failure </t>
+  </si>
+  <si>
+    <t>singleuseradd_student_success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleuseradd_course_head_success </t>
+  </si>
+  <si>
+    <t>singleuseradd_faculty_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_teaching fellow_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_designer_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_teacher_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_guest_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_course_support_staff_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_teaching staff_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_shopper_success</t>
+  </si>
+  <si>
+    <t>singleuseradd_observer_success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,11 +231,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11.3"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,7 +249,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,21 +287,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -210,6 +334,15 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -228,6 +361,15 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,27 +704,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -591,21 +729,21 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>9</v>
@@ -617,15 +755,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -637,15 +775,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -657,34 +795,273 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="4">
+        <v>12345678</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection activeCell="E20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -692,100 +1069,300 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformatted a data field -- test was recognizing it as a float rather than a string. 'float' object has no attribute 'split'
</commit_message>
<xml_diff>
--- a/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
+++ b/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t>test_case_id</t>
   </si>
@@ -64,96 +64,63 @@
     <t>failures expected</t>
   </si>
   <si>
-    <t xml:space="preserve">singleuseradd_student </t>
-  </si>
-  <si>
     <t>aa000fre</t>
   </si>
   <si>
     <t>Student</t>
   </si>
   <si>
-    <t>singleuseradd_course_head</t>
-  </si>
-  <si>
     <t>aa000fsf</t>
   </si>
   <si>
     <t>Course Head</t>
   </si>
   <si>
-    <t>singleuseradd_faculty</t>
-  </si>
-  <si>
     <t>aa000ftg</t>
   </si>
   <si>
     <t>Faculty</t>
   </si>
   <si>
-    <t xml:space="preserve">singleuseradd_teaching fellow </t>
-  </si>
-  <si>
     <t>aa000fuh</t>
   </si>
   <si>
     <t>TA</t>
   </si>
   <si>
-    <t xml:space="preserve">singleuseradd_designer </t>
-  </si>
-  <si>
     <t>aa000fvi</t>
   </si>
   <si>
     <t>Designer</t>
   </si>
   <si>
-    <t>singleuseradd_teacher</t>
-  </si>
-  <si>
     <t>aa000fwj</t>
   </si>
   <si>
     <t>Teacher</t>
   </si>
   <si>
-    <t>singleuseradd_guest</t>
-  </si>
-  <si>
     <t>aa000fxk</t>
   </si>
   <si>
-    <t>singleuseradd_course_support_staff</t>
-  </si>
-  <si>
     <t>aa000fyl</t>
   </si>
   <si>
     <t>Course Support Staff</t>
   </si>
   <si>
-    <t xml:space="preserve">singleuseradd_teaching staff </t>
-  </si>
-  <si>
     <t>aa000fzm</t>
   </si>
   <si>
     <t>Teaching Staff</t>
   </si>
   <si>
-    <t xml:space="preserve">singleuseradd_shopper </t>
-  </si>
-  <si>
     <t>aa000g0l</t>
   </si>
   <si>
     <t>Shopper</t>
   </si>
   <si>
-    <t>singleuseradd_observer</t>
-  </si>
-  <si>
     <t>aa000g1m</t>
   </si>
   <si>
@@ -194,6 +161,9 @@
   </si>
   <si>
     <t>singleuseradd_observer_success</t>
+  </si>
+  <si>
+    <t>12345678</t>
   </si>
 </sst>
 </file>
@@ -249,7 +219,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,17 +275,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -343,6 +320,11 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -370,6 +352,11 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,13 +694,10 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -797,13 +781,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -817,13 +801,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -837,13 +821,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -857,13 +841,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -877,13 +861,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
         <v>7</v>
@@ -897,13 +881,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
@@ -917,10 +901,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -937,13 +921,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
         <v>11</v>
@@ -957,13 +941,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
@@ -977,13 +961,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>14</v>
@@ -997,13 +981,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
         <v>15</v>
@@ -1017,10 +1001,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="4">
-        <v>12345678</v>
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -1048,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="A1:XFD1048576"/>
+      <selection activeCell="E17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1138,13 +1122,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1158,13 +1142,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1178,13 +1162,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -1198,13 +1182,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -1218,13 +1202,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
         <v>7</v>
@@ -1238,13 +1222,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
@@ -1258,10 +1242,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -1278,13 +1262,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
         <v>11</v>
@@ -1298,13 +1282,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
@@ -1318,13 +1302,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>14</v>
@@ -1338,13 +1322,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
         <v>15</v>
@@ -1354,6 +1338,26 @@
       </c>
       <c r="F15">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed shopper role from test data
</commit_message>
<xml_diff>
--- a/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
+++ b/selenium_tests/course_info/test_data/add_people_search_terms.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hic048/projects/canvas_account_admin_tools/selenium_tests/course_info/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15440" yWindow="-21940" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,15 +20,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>test_case_id</t>
   </si>
@@ -691,15 +693,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -959,18 +959,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -979,54 +979,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>9</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1038,9 +1013,9 @@
       <selection activeCell="E17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1080,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1140,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1160,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -1180,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -1200,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1220,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1240,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1260,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1280,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1300,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1320,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -1340,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1363,10 +1338,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>